<commit_message>
files for Liberia parameter estimation
</commit_message>
<xml_diff>
--- a/Information for parameter estimation.xlsx
+++ b/Information for parameter estimation.xlsx
@@ -509,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:H31"/>
+  <dimension ref="B4:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,7 +559,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C17" s="1" t="s">
         <v>21</v>
       </c>
@@ -579,7 +579,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C18" s="1" t="s">
         <v>8</v>
       </c>
@@ -599,7 +599,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C19" s="1" t="s">
         <v>9</v>
       </c>
@@ -618,24 +618,33 @@
       <c r="H19" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="I19">
+        <v>10.548500000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C20" s="6" t="s">
         <v>22</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="I20">
+        <v>0.1769</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C21" s="6" t="s">
         <v>23</v>
       </c>
       <c r="H21" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="I21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C22" s="6" t="s">
         <v>24</v>
       </c>
@@ -643,22 +652,28 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C23" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="I23">
+        <v>7.7999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C24" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="I24">
+        <v>0.68200000000000005</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
         <v>17</v>
       </c>

</xml_diff>